<commit_message>
Mobile App Documents are updated
Mobile App Documents are updated
</commit_message>
<xml_diff>
--- a/SR Smart App/Active/APP_VER_SRSMART_01.01.01.xlsx
+++ b/SR Smart App/Active/APP_VER_SRSMART_01.01.01.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="iOS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="68">
   <si>
     <t>Sr #</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Quick Start Guide</t>
   </si>
   <si>
-    <t>SR Smart Help - 01.01.08</t>
-  </si>
-  <si>
     <t>Release Note</t>
   </si>
   <si>
@@ -194,13 +191,46 @@
   </si>
   <si>
     <t>July 26, 2015</t>
+  </si>
+  <si>
+    <t>01.02.01</t>
+  </si>
+  <si>
+    <t>Sept 18, 2015</t>
+  </si>
+  <si>
+    <t>SR_SMART_HELP</t>
+  </si>
+  <si>
+    <t>Old Keeler Firmware</t>
+  </si>
+  <si>
+    <t>03.01.03</t>
+  </si>
+  <si>
+    <t>02.01.01</t>
+  </si>
+  <si>
+    <t>06.01.01 with EPROM</t>
+  </si>
+  <si>
+    <t>02.01.02 with EPROM</t>
+  </si>
+  <si>
+    <t>03.02.02 with EPROM</t>
+  </si>
+  <si>
+    <t>01.02.02</t>
+  </si>
+  <si>
+    <t>Sept 21, 2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -248,6 +278,12 @@
       <color theme="4"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -290,9 +326,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -331,10 +368,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -348,7 +383,8 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -679,11 +715,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -692,13 +728,14 @@
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="6" max="6" width="40.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" customWidth="1"/>
     <col min="10" max="10" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,11 +761,11 @@
         <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1">
+    <row r="2" spans="1:10" ht="34" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -742,27 +779,49 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="C3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
+      <c r="I3" s="15" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1">
       <c r="A4" s="4"/>
@@ -869,167 +928,220 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="36" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="8" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="43" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="43" customHeight="1">
+      <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="21" customHeight="1"/>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B17" s="16" t="s">
+    <row r="18" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19" spans="2:6" ht="15.75" customHeight="1">
       <c r="B19" s="8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B20" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-    </row>
     <row r="21" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B22" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="B22" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
     </row>
     <row r="23" spans="2:6" ht="15.75" customHeight="1">
       <c r="B23" s="8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>8</v>
+      <c r="C24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="B26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
       <c r="B27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B30" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="16" t="s">
+    <row r="34" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B34" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="10" t="s">
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B35" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="16" t="s">
+      <c r="C35" s="11"/>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B37" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B33" s="12" t="s">
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+    </row>
+    <row r="38" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B38" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C38" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B32:D32"/>
+  <mergeCells count="11">
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B30:D30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1"/>
@@ -1037,10 +1149,14 @@
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="D7" r:id="rId4" display="https://itunes.apple.com/us/app/securemote-smart/id967169177?mt=8"/>
     <hyperlink ref="E7" r:id="rId5" display="https://itunes.apple.com/us/app/securemote-smart/id967169177?mt=8"/>
-    <hyperlink ref="F2" r:id="rId6" tooltip="SR Smart Help - 01.01.08"/>
-    <hyperlink ref="G2" r:id="rId7" tooltip="User Manual"/>
-    <hyperlink ref="H2" r:id="rId8" tooltip="Quick Start Guide"/>
-    <hyperlink ref="I2" r:id="rId9" tooltip="Release Note - iOS"/>
+    <hyperlink ref="F2" r:id="rId6"/>
+    <hyperlink ref="G2" r:id="rId7"/>
+    <hyperlink ref="H2" r:id="rId8"/>
+    <hyperlink ref="I2" r:id="rId9"/>
+    <hyperlink ref="F3" r:id="rId10"/>
+    <hyperlink ref="G3" r:id="rId11"/>
+    <hyperlink ref="H3" r:id="rId12"/>
+    <hyperlink ref="I3" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1054,11 +1170,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1066,14 +1182,15 @@
     <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" customWidth="1"/>
     <col min="10" max="10" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
@@ -1099,7 +1216,7 @@
         <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J1" s="1"/>
     </row>
@@ -1117,27 +1234,49 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="15" t="s">
-        <v>55</v>
+      <c r="I2" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1">
       <c r="A4" s="4"/>
@@ -1170,10 +1309,10 @@
     <row r="7" spans="1:10" ht="75" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -1186,7 +1325,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -1199,7 +1338,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -1244,167 +1383,222 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="51" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="8" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="42" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="50" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="21" customHeight="1"/>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="2:6" ht="21" customHeight="1"/>
+    <row r="18" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19" spans="2:6" ht="15.75" customHeight="1">
       <c r="B19" s="8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B20" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-    </row>
     <row r="21" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B22" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="B22" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
     </row>
     <row r="23" spans="2:6" ht="15.75" customHeight="1">
       <c r="B23" s="8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>8</v>
+      <c r="C24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="B26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
       <c r="B27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B30" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="16" t="s">
+    <row r="34" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B34" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="10" t="s">
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B35" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="16" t="s">
+      <c r="C35" s="11"/>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B37" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B33" s="12" t="s">
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+    </row>
+    <row r="38" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B38" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C38" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B32:D32"/>
+  <mergeCells count="11">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B22:D22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1"/>
@@ -1412,14 +1606,18 @@
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="D7" r:id="rId4" display="https://play.google.com/store/apps/details?id=com.belwith.securemotesmartapp&amp;hl=en"/>
     <hyperlink ref="E7" r:id="rId5" display="https://play.google.com/store/apps/details?id=com.belwith.securemotesmartapp&amp;hl=en"/>
-    <hyperlink ref="F2" r:id="rId6" tooltip="SR Smart Help - 01.01.08"/>
-    <hyperlink ref="G2" r:id="rId7" tooltip="User Manual"/>
-    <hyperlink ref="H2" r:id="rId8" tooltip="Quick Start Guide"/>
-    <hyperlink ref="I2" r:id="rId9" tooltip="Release Note - Android"/>
-    <hyperlink ref="D8" r:id="rId10" display="https://www.delphiansystems.com/sr/android/"/>
-    <hyperlink ref="E8" r:id="rId11" display="https://www.delphiansystems.com/sr/android/"/>
-    <hyperlink ref="D9" r:id="rId12" display="http://integration.belwith.com/appstaging/InstallAppsAndroid.html"/>
-    <hyperlink ref="E9" r:id="rId13" display="http://integration.belwith.com/appstaging/InstallAppsAndroid.html"/>
+    <hyperlink ref="D8" r:id="rId6" display="https://www.delphiansystems.com/sr/android/"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://www.delphiansystems.com/sr/android/"/>
+    <hyperlink ref="D9" r:id="rId8" display="http://integration.belwith.com/appstaging/InstallAppsAndroid.html"/>
+    <hyperlink ref="E9" r:id="rId9" display="http://integration.belwith.com/appstaging/InstallAppsAndroid.html"/>
+    <hyperlink ref="F2" r:id="rId10"/>
+    <hyperlink ref="G2" r:id="rId11"/>
+    <hyperlink ref="H2" r:id="rId12"/>
+    <hyperlink ref="I2" r:id="rId13"/>
+    <hyperlink ref="F3" r:id="rId14"/>
+    <hyperlink ref="G3" r:id="rId15"/>
+    <hyperlink ref="H3" r:id="rId16"/>
+    <hyperlink ref="I3" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>